<commit_message>
Ran program created extra files
</commit_message>
<xml_diff>
--- a/excel/stray_2021.xlsx
+++ b/excel/stray_2021.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD84FE2-3E15-4A05-A3BE-FE870D1D3FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D236D91A-2017-4EAD-93FA-DAAA73B60950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42960" yWindow="1275" windowWidth="14415" windowHeight="7815" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hour_register" sheetId="1" r:id="rId1"/>
     <sheet name="1" sheetId="2" r:id="rId2"/>
     <sheet name="2" sheetId="3" r:id="rId3"/>
-    <sheet name="Students" sheetId="4" r:id="rId4"/>
-    <sheet name="Costumers" sheetId="5" r:id="rId5"/>
-    <sheet name="Company" sheetId="6" r:id="rId6"/>
+    <sheet name="3" sheetId="4" r:id="rId4"/>
+    <sheet name="4" sheetId="5" r:id="rId5"/>
+    <sheet name="5" sheetId="6" r:id="rId6"/>
+    <sheet name="6" sheetId="7" r:id="rId7"/>
+    <sheet name="7" sheetId="8" r:id="rId8"/>
+    <sheet name="8" sheetId="9" r:id="rId9"/>
+    <sheet name="9" sheetId="10" r:id="rId10"/>
+    <sheet name="10" sheetId="11" r:id="rId11"/>
+    <sheet name="11" sheetId="12" r:id="rId12"/>
+    <sheet name="12" sheetId="13" r:id="rId13"/>
+    <sheet name="Students" sheetId="14" r:id="rId14"/>
+    <sheet name="Costumers" sheetId="15" r:id="rId15"/>
+    <sheet name="Company" sheetId="16" r:id="rId16"/>
+    <sheet name="Rental" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +72,15 @@
     <t>03.02.2021</t>
   </si>
   <si>
+    <t>08.02.2021</t>
+  </si>
+  <si>
+    <t>10.02.2021</t>
+  </si>
+  <si>
+    <t>15.02.2021</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -103,6 +123,18 @@
     <t>anetteengerevensen@gmail.com</t>
   </si>
   <si>
+    <t>Nora Bull</t>
+  </si>
+  <si>
+    <t>nora.bull.langehaug@outlook.com</t>
+  </si>
+  <si>
+    <t>Hannah Schonemann</t>
+  </si>
+  <si>
+    <t>hasc1450@gmail.com; schonemanhannah@gmail.com</t>
+  </si>
+  <si>
     <t>Adress</t>
   </si>
   <si>
@@ -151,16 +183,25 @@
     <t>1506.42.37524</t>
   </si>
   <si>
-    <t>Nora Bull</t>
-  </si>
-  <si>
-    <t>hasc1450@gmail.com; schonemanhannah@gmail.com</t>
-  </si>
-  <si>
-    <t>Hannah Schonemann</t>
-  </si>
-  <si>
-    <t>nora.bull.langehaug@outlook.com</t>
+    <t>Nedbetaling</t>
+  </si>
+  <si>
+    <t>Utleie snowboard dag</t>
+  </si>
+  <si>
+    <t>Utleie snowboard helg</t>
+  </si>
+  <si>
+    <t>Utleie snowboard uke</t>
+  </si>
+  <si>
+    <t>Utleie skredsøker dag</t>
+  </si>
+  <si>
+    <t>Utleie skredsøker helg</t>
+  </si>
+  <si>
+    <t>Utleie skredsøker uke</t>
   </si>
 </sst>
 </file>
@@ -277,14 +318,14 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -601,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,16 +657,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -673,186 +714,107 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K2"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <f>SUM(hour_register!B2)</f>
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>247.5</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>B2*C2</f>
-        <v>495</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f>E2*F2</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f>E2+G2</f>
-        <v>495</v>
-      </c>
-      <c r="I2" s="3">
-        <v>44228</v>
-      </c>
-      <c r="J2">
-        <f>H2</f>
-        <v>495</v>
-      </c>
-      <c r="K2" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <f>SUM(hour_register!B3:B4)</f>
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>247.5</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>B2*C2</f>
-        <v>742.5</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f>E2*F2</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f>E2+G2</f>
-        <v>742.5</v>
-      </c>
-      <c r="I2" s="3">
-        <v>44228</v>
-      </c>
-      <c r="J2" s="2">
-        <f>H2</f>
-        <v>742.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,10 +828,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -877,35 +839,38 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>95338955</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>95493224</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>92270270</v>
@@ -913,22 +878,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId4" display="hasc1450@gmail.com" xr:uid="{31D55AE2-ADDF-4516-A3A0-8EAC5F23D216}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{F7BF6BEB-DA36-41C7-9B64-E616AF6B989A}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="hasc1450@gmail.com" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0D00-000004000000}"/>
+    <hyperlink ref="C4" r:id="rId6" display="hasc1450@gmail.com" xr:uid="{00000000-0004-0000-0D00-000005000000}"/>
+    <hyperlink ref="C2" r:id="rId7" xr:uid="{00000000-0004-0000-0D00-000006000000}"/>
+    <hyperlink ref="C3" r:id="rId8" xr:uid="{00000000-0004-0000-0D00-000007000000}"/>
+    <hyperlink ref="C4" r:id="rId9" display="hasc1450@gmail.com" xr:uid="{00000000-0004-0000-0D00-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -946,19 +915,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -966,40 +935,46 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <f>A2+1</f>
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1008,22 +983,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1031,28 +1006,440 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G2">
         <v>924881682</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1">
+        <f>1500-J2</f>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>B2*C2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>E2*F2</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>E2+G2</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44256</v>
+      </c>
+      <c r="J2">
+        <f>SUM(H2:H4)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>B3*C3</f>
+        <v>200</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>E3*F3</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>E3+G3</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>400</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>B4*C4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>E4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>E4+G4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <f>SUM(hour_register!B2)</f>
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>247.5</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>B2*C2</f>
+        <v>495</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>E2*F2</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>E2+G2</f>
+        <v>495</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44228</v>
+      </c>
+      <c r="J2">
+        <f>H2</f>
+        <v>495</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <f>SUM(hour_register!B3:B7)</f>
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>247.5</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>B2*C2</f>
+        <v>1980</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>E2*F2</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>E2+G2</f>
+        <v>1980</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44256</v>
+      </c>
+      <c r="J2" s="2">
+        <f>H2</f>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F3" s="8"/>
+      <c r="I3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>